<commit_message>
Finished custom single cell function
</commit_message>
<xml_diff>
--- a/CH-106 Custom Rank.xlsx
+++ b/CH-106 Custom Rank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FD0F82-FB75-4A72-B4B1-5ADC488FDAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13720C4-5A6B-46EB-93B2-3264B83A7587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1370,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6C9A49-AEBD-41CD-8B20-F3AC34CC554D}">
-  <dimension ref="B1:P28"/>
+  <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1695,6 +1695,16 @@
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I19" s="13" t="str" cm="1">
+        <f t="array" ref="I19:J29">_xlfn.LET(
+_xlpm.d,_xlfn.TAKE(_xlfn._xlws.SORT(C3:G12,{2,3,4},{-1,-1,-1}),,1),
+_xlfn.VSTACK(L2:M2,_xlfn.HSTACK(_xlfn.SEQUENCE(ROWS(_xlpm.d)),_xlpm.d))
+)</f>
+        <v>Rank</v>
+      </c>
+      <c r="J19" s="13" t="str">
+        <v>Country</v>
+      </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
@@ -1709,6 +1719,12 @@
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I20" s="12">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8" t="str">
+        <v>USA</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -1723,6 +1739,12 @@
       <c r="E21" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I21" s="12">
+        <v>2</v>
+      </c>
+      <c r="J21" s="8" t="str">
+        <v>China</v>
+      </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
@@ -1737,6 +1759,12 @@
       <c r="E22" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I22" s="12">
+        <v>3</v>
+      </c>
+      <c r="J22" s="8" t="str">
+        <v>Japan</v>
+      </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
@@ -1751,6 +1779,12 @@
       <c r="E23" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I23" s="12">
+        <v>4</v>
+      </c>
+      <c r="J23" s="8" t="str">
+        <v>Australia</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
@@ -1765,6 +1799,12 @@
       <c r="E24" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I24" s="12">
+        <v>5</v>
+      </c>
+      <c r="J24" s="8" t="str">
+        <v>France</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
@@ -1779,6 +1819,12 @@
       <c r="E25" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I25" s="12">
+        <v>6</v>
+      </c>
+      <c r="J25" s="8" t="str">
+        <v>Netherlands</v>
+      </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
@@ -1793,6 +1839,12 @@
       <c r="E26" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I26" s="12">
+        <v>7</v>
+      </c>
+      <c r="J26" s="8" t="str">
+        <v>Great Britain</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
@@ -1807,6 +1859,12 @@
       <c r="E27" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I27" s="12">
+        <v>8</v>
+      </c>
+      <c r="J27" s="8" t="str">
+        <v>Republic of Korea</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
@@ -1820,6 +1878,20 @@
       </c>
       <c r="E28" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="I28" s="12">
+        <v>9</v>
+      </c>
+      <c r="J28" s="8" t="str">
+        <v>italy</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I29" s="12">
+        <v>10</v>
+      </c>
+      <c r="J29" s="8" t="str">
+        <v>Germany</v>
       </c>
     </row>
   </sheetData>

</xml_diff>